<commit_message>
Framework - SkillView 수정(View 이름은 임시)
Tab으로 분류할 Category를 기준으로 Dictionary로 Caching -> View List 오브젝트 풀 만들때, 유저 데이터와 비교 갱신 필요
</commit_message>
<xml_diff>
--- a/ExcelToJson/Excel/Skill.xlsx
+++ b/ExcelToJson/Excel/Skill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C\OneDrive\바탕 화면\포트폴리오\Portfolio\ExcelToJson\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884280D0-88D6-4EDA-93A1-A3D8055C8101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD6168F-B258-4D14-8FB1-2A31D66A7C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56640" yWindow="165" windowWidth="28950" windowHeight="15510" xr2:uid="{D3830896-87BE-45CE-B29F-286ABAF8FA2F}"/>
+    <workbookView xWindow="57390" yWindow="0" windowWidth="28950" windowHeight="15510" xr2:uid="{D3830896-87BE-45CE-B29F-286ABAF8FA2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="1" r:id="rId1"/>
@@ -56,10 +56,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ShopID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -393,6 +389,10 @@
   </si>
   <si>
     <t>EARTH</t>
+  </si>
+  <si>
+    <t>SkillID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -860,7 +860,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -881,16 +881,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -901,36 +901,36 @@
         <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -938,19 +938,19 @@
         <v>50001</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -958,19 +958,19 @@
         <v>50002</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -978,19 +978,19 @@
         <v>50003</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -998,19 +998,19 @@
         <v>50004</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" s="9">
         <v>1</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -1018,19 +1018,19 @@
         <v>50005</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -1038,19 +1038,19 @@
         <v>50006</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -1058,19 +1058,19 @@
         <v>50007</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -1078,19 +1078,19 @@
         <v>50008</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -1098,19 +1098,19 @@
         <v>50009</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -1118,19 +1118,19 @@
         <v>50010</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -1138,19 +1138,19 @@
         <v>50011</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
@@ -1158,19 +1158,19 @@
         <v>50012</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
@@ -1178,19 +1178,19 @@
         <v>50013</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1198,19 +1198,19 @@
         <v>50014</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -1218,19 +1218,19 @@
         <v>50015</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -1238,19 +1238,19 @@
         <v>50016</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -1258,19 +1258,19 @@
         <v>50017</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
@@ -1278,19 +1278,19 @@
         <v>50018</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
@@ -1298,19 +1298,19 @@
         <v>50019</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
@@ -1318,19 +1318,19 @@
         <v>50020</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
@@ -1338,19 +1338,19 @@
         <v>50021</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
@@ -1358,19 +1358,19 @@
         <v>50022</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1378,19 +1378,19 @@
         <v>50023</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1398,19 +1398,19 @@
         <v>50024</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -1418,19 +1418,19 @@
         <v>50025</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -1438,19 +1438,19 @@
         <v>50026</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -1458,19 +1458,19 @@
         <v>50027</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -1478,19 +1478,19 @@
         <v>50028</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -1498,19 +1498,19 @@
         <v>50029</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>